<commit_message>
Revision finish, update production file
</commit_message>
<xml_diff>
--- a/hardware/main/kicad/production/TeapotLabsBWLR1F_BOM.xlsx
+++ b/hardware/main/kicad/production/TeapotLabsBWLR1F_BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main Storage\03_Work\04_Teapot Laboratories\bwlr1f\hardware\main\kicad\production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Main Storage\03_Work\04_Teapot Laboratories\bwlr1f\hardware\main\kicad\production_old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BB860F-4FF2-44F6-BA5D-77C2548345E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF22356-2475-445D-B4A3-FBC9E31C4CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{7C79802E-C84C-4FEC-9587-CFA1B72D0FA2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="BOM (2)" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'BOM (2)'!$A$1:$M$36</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'BOM (2)'!$A$1:$M$35</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="198">
   <si>
     <t>Id</t>
   </si>
@@ -310,30 +310,6 @@
   </si>
   <si>
     <t>https://www.lcsc.com/datasheet/lcsc_datasheet_1808311544_WILLSEMI-Will-Semicon-ESD5651N-2-TR_C239784.pdf</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>TE Connectivity Linx</t>
-  </si>
-  <si>
-    <t>ANT-915-USP410</t>
-  </si>
-  <si>
-    <t>RF Ant 915 MHz Chip Solder SMD</t>
-  </si>
-  <si>
-    <t>bwlr1f:XDCR_ANT-915-USP410</t>
-  </si>
-  <si>
-    <t>343-ANT-915-USP410CT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-linx/ANT-915-USP410/13165344</t>
-  </si>
-  <si>
-    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=ant-915-usp410-ds&amp;DocType=Data+Sheet&amp;DocLang=English&amp;DocFormat=pdf&amp;PartCntxt=ANT-915-USP410</t>
   </si>
   <si>
     <t>L1,L3,L4</t>
@@ -1261,8 +1237,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54F57BD8-B214-4498-A6E6-67C2F8725BAA}" name="BOM" displayName="BOM" ref="A1:M36" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:M36" xr:uid="{54F57BD8-B214-4498-A6E6-67C2F8725BAA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{54F57BD8-B214-4498-A6E6-67C2F8725BAA}" name="BOM" displayName="BOM" ref="A1:M35" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:M35" xr:uid="{54F57BD8-B214-4498-A6E6-67C2F8725BAA}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{D5D72330-C512-4D2E-9CD4-44453A950121}" uniqueName="1" name="Id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{413537D3-6D78-412E-AACC-49154B523B15}" uniqueName="2" name="Designator" queryTableFieldId="2" dataDxfId="10"/>
@@ -1579,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EE39AA4-5573-4D69-AC5C-EFB339AB88E5}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2060,7 +2036,7 @@
         <v>93</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
         <v>94</v>
@@ -2069,28 +2045,28 @@
         <v>95</v>
       </c>
       <c r="F12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="I12" t="s">
         <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -2098,25 +2074,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" t="s">
         <v>102</v>
       </c>
-      <c r="E13" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" t="s">
-        <v>104</v>
-      </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>188</v>
       </c>
       <c r="H13" t="s">
-        <v>106</v>
+        <v>190</v>
       </c>
       <c r="I13" t="s">
         <v>19</v>
@@ -2125,13 +2101,13 @@
         <v>20</v>
       </c>
       <c r="K13" t="s">
-        <v>107</v>
-      </c>
-      <c r="L13" t="s">
-        <v>108</v>
-      </c>
-      <c r="M13" t="s">
-        <v>109</v>
+        <v>192</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -2139,40 +2115,40 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>193</v>
-      </c>
-      <c r="E14" t="s">
-        <v>195</v>
+        <v>186</v>
+      </c>
+      <c r="E14" s="2">
+        <v>74404042150</v>
       </c>
       <c r="F14" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H14" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="I14" t="s">
         <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="K14" t="s">
-        <v>200</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>202</v>
+        <v>195</v>
+      </c>
+      <c r="L14" t="s">
+        <v>196</v>
+      </c>
+      <c r="M14" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
@@ -2180,40 +2156,40 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>191</v>
+        <v>103</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
-      </c>
-      <c r="E15" s="2">
-        <v>74404042150</v>
+        <v>104</v>
+      </c>
+      <c r="E15" t="s">
+        <v>105</v>
       </c>
       <c r="F15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G15" t="s">
-        <v>197</v>
+        <v>107</v>
       </c>
       <c r="H15" t="s">
-        <v>199</v>
+        <v>108</v>
       </c>
       <c r="I15" t="s">
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="K15" t="s">
-        <v>203</v>
+        <v>109</v>
       </c>
       <c r="L15" t="s">
-        <v>204</v>
+        <v>110</v>
       </c>
       <c r="M15" t="s">
-        <v>205</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
@@ -2221,25 +2197,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I16" t="s">
         <v>19</v>
@@ -2248,13 +2224,13 @@
         <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="L16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.4">
@@ -2262,13 +2238,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
         <v>122</v>
@@ -2280,7 +2256,7 @@
         <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I17" t="s">
         <v>19</v>
@@ -2289,13 +2265,13 @@
         <v>20</v>
       </c>
       <c r="K17" t="s">
+        <v>125</v>
+      </c>
+      <c r="L17" t="s">
         <v>126</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>127</v>
-      </c>
-      <c r="M17" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.4">
@@ -2303,25 +2279,25 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
         <v>129</v>
       </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>130</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>131</v>
       </c>
-      <c r="G18" t="s">
-        <v>132</v>
-      </c>
       <c r="H18" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I18" t="s">
         <v>19</v>
@@ -2330,13 +2306,13 @@
         <v>20</v>
       </c>
       <c r="K18" t="s">
+        <v>132</v>
+      </c>
+      <c r="L18" t="s">
         <v>133</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>134</v>
-      </c>
-      <c r="M18" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.4">
@@ -2344,25 +2320,25 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" t="s">
         <v>137</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>138</v>
       </c>
-      <c r="G19" t="s">
-        <v>139</v>
-      </c>
       <c r="H19" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="I19" t="s">
         <v>19</v>
@@ -2371,13 +2347,13 @@
         <v>20</v>
       </c>
       <c r="K19" t="s">
+        <v>139</v>
+      </c>
+      <c r="L19" t="s">
         <v>140</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>141</v>
-      </c>
-      <c r="M19" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.4">
@@ -2385,13 +2361,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>143</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>121</v>
       </c>
       <c r="E20" t="s">
         <v>144</v>
@@ -2400,25 +2376,25 @@
         <v>145</v>
       </c>
       <c r="G20" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" t="s">
         <v>146</v>
-      </c>
-      <c r="H20" t="s">
-        <v>125</v>
       </c>
       <c r="I20" t="s">
         <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>20</v>
+        <v>143</v>
       </c>
       <c r="K20" t="s">
+        <v>144</v>
+      </c>
+      <c r="L20" t="s">
         <v>147</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>148</v>
-      </c>
-      <c r="M20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.4">
@@ -2426,34 +2402,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
         <v>151</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
+        <v>151</v>
+      </c>
+      <c r="G21" t="s">
         <v>152</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>153</v>
-      </c>
-      <c r="G21" t="s">
-        <v>153</v>
-      </c>
-      <c r="H21" t="s">
-        <v>154</v>
       </c>
       <c r="I21" t="s">
         <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>151</v>
+        <v>60</v>
       </c>
       <c r="K21" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="L21" t="s">
         <v>155</v>
@@ -2479,28 +2455,28 @@
         <v>159</v>
       </c>
       <c r="F22" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G22" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H22" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I22" t="s">
         <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="L22" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="M22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
@@ -2508,16 +2484,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E23" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F23" t="s">
         <v>168</v>
@@ -2532,7 +2508,7 @@
         <v>19</v>
       </c>
       <c r="J23" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="K23" t="s">
         <v>171</v>
@@ -2561,75 +2537,34 @@
         <v>176</v>
       </c>
       <c r="F24" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="I24" t="s">
         <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="K24" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="L24" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="M24" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
         <v>182</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>183</v>
-      </c>
-      <c r="E25" t="s">
-        <v>184</v>
-      </c>
-      <c r="F25" t="s">
-        <v>185</v>
-      </c>
-      <c r="G25" t="s">
-        <v>186</v>
-      </c>
-      <c r="H25" t="s">
-        <v>187</v>
-      </c>
-      <c r="I25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" t="s">
-        <v>20</v>
-      </c>
-      <c r="K25" t="s">
-        <v>188</v>
-      </c>
-      <c r="L25" t="s">
-        <v>189</v>
-      </c>
-      <c r="M25" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L14" r:id="rId1" xr:uid="{D6A318D1-1F48-4DBB-936F-C8EF74CD45FD}"/>
-    <hyperlink ref="M14" r:id="rId2" xr:uid="{240FD9AF-9C3C-48B3-97DE-CF6690BE4DD3}"/>
+    <hyperlink ref="L13" r:id="rId1" xr:uid="{D6A318D1-1F48-4DBB-936F-C8EF74CD45FD}"/>
+    <hyperlink ref="M13" r:id="rId2" xr:uid="{240FD9AF-9C3C-48B3-97DE-CF6690BE4DD3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>